<commit_message>
Sensor Interfacing Done-Second Evalution
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Progress Report</t>
   </si>
@@ -37,7 +37,13 @@
     <t xml:space="preserve">Ashish Bhardwaj</t>
   </si>
   <si>
+    <t xml:space="preserve">Poonam Devkar</t>
+  </si>
+  <si>
     <t xml:space="preserve">project evaluation and sensor interfacing (temperature and humidity sensor DHT22) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current sensor(INA219) interfacing using I2C protocol.</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,7 +351,9 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
@@ -354,9 +362,11 @@
         <v>45303</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>

</xml_diff>